<commit_message>
add unit test for refugee
</commit_message>
<xml_diff>
--- a/model/data/refugee/xlsx/refugee.xlsx
+++ b/model/data/refugee/xlsx/refugee.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tdijk004/Documents/Tooling/tRBS/open source/trbs-refugee/trbs/model/data/refugee/xlsx/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tdijk004/Documents/Tooling/tRBS/open source/trbs-refugee-2/trbs-add-refugee/model/data/refugee/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27AA6B37-6044-DD4E-9F5B-56D3D9AB092F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E89EA71-60BF-0F4C-A7C6-D577FEDFF97E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="860" yWindow="2460" windowWidth="31660" windowHeight="15880" activeTab="5" xr2:uid="{4D223BC5-A265-7B41-9F5C-066E948A074C}"/>
   </bookViews>
@@ -603,7 +603,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -625,12 +625,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -662,7 +656,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -671,7 +665,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -2189,8 +2182,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45498073-CC56-2D41-B5D6-3D03F1233978}">
   <dimension ref="A1:H98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2513,11 +2506,10 @@
       <c r="A20" t="s">
         <v>105</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5" t="s">
+      <c r="D20" t="s">
         <v>167</v>
       </c>
       <c r="E20">
@@ -2814,16 +2806,16 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="5" t="s">
+      <c r="A41" t="s">
         <v>127</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="B41" t="s">
         <v>40</v>
       </c>
-      <c r="C41" s="5" t="s">
+      <c r="C41" t="s">
         <v>41</v>
       </c>
-      <c r="D41" s="5" t="s">
+      <c r="D41" t="s">
         <v>168</v>
       </c>
     </row>
@@ -3094,16 +3086,16 @@
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A61" s="6" t="s">
+      <c r="A61" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="B61" s="6" t="s">
+      <c r="B61" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C61" s="6" t="s">
+      <c r="C61" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="D61" s="6" t="s">
+      <c r="D61" s="5" t="s">
         <v>164</v>
       </c>
     </row>

</xml_diff>